<commit_message>
experiment update communication cost
</commit_message>
<xml_diff>
--- a/experiment0302.xlsx
+++ b/experiment0302.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="96">
   <si>
     <t>parallelism</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -381,6 +381,27 @@
     <t>ε</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>communication cost(between mapper and reducer, K bytes sent)</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>sendv</t>
+  </si>
+  <si>
+    <t>basic-s</t>
+  </si>
+  <si>
+    <t>improved-s</t>
+  </si>
+  <si>
+    <t>twoLevel-s</t>
+  </si>
+  <si>
+    <t>ε</t>
+  </si>
 </sst>
 </file>
 
@@ -402,15 +423,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -418,14 +445,114 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2761,6 +2888,1034 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>communication cost(K bytes sent)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>communication cost(between mapper and reducer, K bytes sent)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$45:$F$46</c:f>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$47:$F$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2726-461D-97E4-C8A04E16B3D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$45:$F$46</c:f>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$48:$F$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2726-461D-97E4-C8A04E16B3D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$45:$F$46</c:f>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$49:$F$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2726-461D-97E4-C8A04E16B3D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sendv</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$45:$F$46</c:f>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$50:$F$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9531555</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9531555</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9531555</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9531555</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9531555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2726-461D-97E4-C8A04E16B3D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1237665231"/>
+        <c:axId val="1239643743"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1237665231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1239643743"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1239643743"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1237665231"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>communication cost(K bytes sent)</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15491886894704965"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$54</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>communication cost(between mapper and reducer, K bytes sent)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$52:$E$53</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>714</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>704</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>720</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>705</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$54:$E$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C4FC-4DA0-99C9-E3CCE4AE5DD4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$52:$E$53</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>714</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>704</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>720</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>705</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$55:$E$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C4FC-4DA0-99C9-E3CCE4AE5DD4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$52:$E$53</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>714</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>704</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>720</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>705</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$56:$E$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C4FC-4DA0-99C9-E3CCE4AE5DD4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1237671055"/>
+        <c:axId val="1299205439"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1237671055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1299205439"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1299205439"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1237671055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2921,6 +4076,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4470,6 +5705,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5393,6 +7660,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{077006D0-EFA4-4935-8FC8-E23410409E13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{462CBA05-FBEB-4D80-A146-FD1370A007C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7403,10 +9746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7551,371 +9894,594 @@
         <v xml:space="preserve">/share/flink/tmp/freqs/dataset245freq.txt /share/flink/tmp/freqs/improvedsk30e4coeffreq.txt  /share/flink/tmp/improvedsk30e4sse.txt </v>
       </c>
     </row>
+    <row r="18" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B20">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6">
         <v>10</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="6">
         <v>20</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="6">
         <v>30</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="6">
         <v>40</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="7">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="6">
         <v>1800</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>1860</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>1855</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="6">
         <v>1907</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="7">
         <v>1840</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="6">
         <v>731</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>822</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="6">
         <v>610</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="6">
         <v>609</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="7">
         <v>637</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="6">
         <v>558</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>550</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <v>538</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="6">
         <v>542</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="7">
         <v>536</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="9">
         <v>760</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="9">
         <v>484</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="9">
         <v>502</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="9">
         <v>668</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="10">
         <v>509</v>
       </c>
     </row>
+    <row r="25" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
       <c r="B26" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="F26" s="16"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B27">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6">
         <v>10</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <v>20</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="6">
         <v>30</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="6">
         <v>40</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="7">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="6">
         <v>700062878179</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="6">
         <v>583796393311</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="6">
         <v>572219126720</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="6">
         <v>550712093674</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="7">
         <v>544444457240</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="6">
         <v>701201023371</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <v>585087116118</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="6">
         <v>573524349366</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="6">
         <v>553686184134</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="7">
         <v>545792371032</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="6">
         <v>702153860976</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="6">
         <v>584306725090</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="6">
         <v>554247600964</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="6">
         <v>547810006561</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="7">
         <v>535607820286</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="9">
         <v>700911821068</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="9">
         <v>641819667007</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="9">
         <v>661022747985</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="9">
         <v>656251133849</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="10">
         <v>613990735498</v>
       </c>
     </row>
+    <row r="32" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
       <c r="B33" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="E33" s="16"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B34">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6">
         <v>0.1</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="6">
         <v>0.01</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="7">
         <v>1E-4</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="6">
         <v>355</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="6">
         <v>386</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="6">
         <v>462</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="7">
         <v>610</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="6">
         <v>521</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="6">
         <v>461</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="6">
         <v>496</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="7">
         <v>538</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="9">
         <v>528</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="9">
         <v>521</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="9">
         <v>623</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="10">
         <v>502</v>
       </c>
     </row>
+    <row r="38" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
       <c r="B39" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="E39" s="16"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B40">
+      <c r="A40" s="5"/>
+      <c r="B40" s="6">
         <v>0.1</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="6">
         <v>0.01</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="7">
         <v>1E-4</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="6">
         <v>2686616258304760</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="6">
         <v>1643963023519</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="6">
         <v>573181449951</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="7">
         <v>573524349366</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="6">
         <v>2735284001304760</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="6">
         <v>1479305784769</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="6">
         <v>776794331363</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="7">
         <v>554247600964</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="43" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="9">
         <v>1.09352701583047E+16</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="9">
         <v>71407816464769</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="9">
         <v>1807026300605</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="10">
         <v>661022747985</v>
       </c>
     </row>
+    <row r="46" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="4"/>
+      <c r="B48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="16"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="11"/>
+      <c r="B49" s="6">
+        <v>10</v>
+      </c>
+      <c r="C49" s="6">
+        <v>20</v>
+      </c>
+      <c r="D49" s="6">
+        <v>30</v>
+      </c>
+      <c r="E49" s="6">
+        <v>40</v>
+      </c>
+      <c r="F49" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="12">
+        <v>9531555</v>
+      </c>
+      <c r="C50" s="12">
+        <v>9531555</v>
+      </c>
+      <c r="D50" s="12">
+        <v>9531555</v>
+      </c>
+      <c r="E50" s="12">
+        <v>9531555</v>
+      </c>
+      <c r="F50" s="15">
+        <v>9531555</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="12">
+        <v>1132462</v>
+      </c>
+      <c r="C51" s="12">
+        <v>1132462</v>
+      </c>
+      <c r="D51" s="12">
+        <v>1132462</v>
+      </c>
+      <c r="E51" s="12">
+        <v>1132462</v>
+      </c>
+      <c r="F51" s="15">
+        <v>1132462</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B52" s="12">
+        <v>3</v>
+      </c>
+      <c r="C52" s="12">
+        <v>3</v>
+      </c>
+      <c r="D52" s="12">
+        <v>3</v>
+      </c>
+      <c r="E52" s="12">
+        <v>3</v>
+      </c>
+      <c r="F52" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="9">
+        <v>714</v>
+      </c>
+      <c r="C53" s="9">
+        <v>704</v>
+      </c>
+      <c r="D53" s="9">
+        <v>720</v>
+      </c>
+      <c r="E53" s="9">
+        <v>705</v>
+      </c>
+      <c r="F53" s="10">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="4"/>
+      <c r="B55" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="13"/>
+      <c r="B56" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C56" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="D56" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="E56" s="7">
+        <v>1E-4</v>
+      </c>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="12">
+        <v>2.87</v>
+      </c>
+      <c r="C57" s="12">
+        <v>118</v>
+      </c>
+      <c r="D57" s="12">
+        <v>11776</v>
+      </c>
+      <c r="E57" s="15">
+        <v>1132462</v>
+      </c>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="12">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="C58" s="12">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D58" s="12">
+        <v>0.192</v>
+      </c>
+      <c r="E58" s="7">
+        <v>3</v>
+      </c>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="9">
+        <v>1.32</v>
+      </c>
+      <c r="C59" s="9">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="D59" s="9">
+        <v>75.5</v>
+      </c>
+      <c r="E59" s="10">
+        <v>720</v>
+      </c>
+      <c r="F59" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B48:F48"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>